<commit_message>
xs schema process start
</commit_message>
<xml_diff>
--- a/src/main/resources/DemoXml/Xml File Info.xlsx
+++ b/src/main/resources/DemoXml/Xml File Info.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nabeel.Ahmed\Desktop\Demo Xml\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nabeel.Ahmed\Downloads\RAAD-Converter\src\main\resources\DemoXml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37953A1A-BBC1-4147-8889-641630FC75C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDED9166-DBED-4866-9BB3-5E7E1C12DC5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Xml Tage With Key" sheetId="1" r:id="rId1"/>
+    <sheet name="XML Schema Definition (XSD)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,8 +25,67 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Nabeel Ahmed Jamil</author>
+  </authors>
+  <commentList>
+    <comment ref="B21" authorId="0" shapeId="0" xr:uid="{5941E0F8-BE65-4AA7-853B-A41AD476B726}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nabeel Ahmed Jamil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+elements and data types used in the schema come from this link, and
+namespace should be prefixed with xs:</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B22" authorId="0" shapeId="0" xr:uid="{CAB5B811-7579-4F4B-A24B-5EE42B8D5154}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nabeel Ahmed Jamil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+indicates that any elements used by the XML instance document which were declared in this schema must be namespace qualified</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>http://www.globenewswire.com/news-release/2020/02/13/1984375/0/en/Magnetic-Resonance-Imaging-MRI-Devices-and-Equipment-Industry-2015-2030-Global-Market-to-Reach-9-34B-by-2022-Rising-from-7-6B-in-2018.html</t>
   </si>
@@ -70,13 +130,110 @@
   </si>
   <si>
     <t>#content-L2 &gt; span &gt; pre</t>
+  </si>
+  <si>
+    <t>&lt;?xml version="1.0"?&gt;
+&lt;xs:schema xmlns:xs="http://www.w3.org/2001/XMLSchema"&gt;
+&lt;xs:element name="note"&gt;
+  &lt;xs:complexType&gt;
+    &lt;xs:sequence&gt;
+      &lt;xs:element name="to" type="xs:string"/&gt;
+      &lt;xs:element name="from" type="xs:string"/&gt;
+      &lt;xs:element name="heading" type="xs:string"/&gt;
+      &lt;xs:element name="body" type="xs:string"/&gt;
+    &lt;/xs:sequence&gt;
+  &lt;/xs:complexType&gt;
+&lt;/xs:element&gt;
+&lt;/xs:schema&gt;</t>
+  </si>
+  <si>
+    <t>Sample XSD</t>
+  </si>
+  <si>
+    <t>Sample XSD OUT-PUT</t>
+  </si>
+  <si>
+    <t>&lt;?xml version="1.0"?&gt;
+&lt;note&gt;
+  &lt;to&gt;Tove&lt;/to&gt;
+  &lt;from&gt;Jani&lt;/from&gt;
+  &lt;heading&gt;Reminder&lt;/heading&gt;
+  &lt;body&gt;Don't forget me this weekend!&lt;/body&gt;
+&lt;/note&gt;</t>
+  </si>
+  <si>
+    <t>&lt;schema&gt; element is the root element of every XML Schema</t>
+  </si>
+  <si>
+    <t>Info</t>
+  </si>
+  <si>
+    <r>
+      <t>xmlns:xs=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFA52A2A"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"http://www.w3.org/2001/XMLSchema"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>elementFormDefault=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFA52A2A"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"qualified"</t>
+    </r>
+  </si>
+  <si>
+    <t>xs:string</t>
+  </si>
+  <si>
+    <t>xs:decimal</t>
+  </si>
+  <si>
+    <t>xs:integer</t>
+  </si>
+  <si>
+    <t>xs:boolean</t>
+  </si>
+  <si>
+    <t>xs:date</t>
+  </si>
+  <si>
+    <t>xs:time</t>
+  </si>
+  <si>
+    <t>Data-Type</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>fixed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,8 +249,72 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFA52A2A"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000CD"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -106,8 +327,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -130,12 +369,92 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -146,6 +465,58 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -429,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,4 +880,386 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{708AC2AB-D2B5-4AF4-BD65-D93FFA26CDBB}">
+  <dimension ref="A1:L28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+    </row>
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="12"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="15"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="15"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="15"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="15"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="15"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="15"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="15"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="15"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="15"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="15"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="15"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="15"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="15"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="15"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="15"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="18"/>
+    </row>
+    <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="22"/>
+      <c r="E23" s="23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="21"/>
+      <c r="E24" s="23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="21"/>
+      <c r="E25" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="21"/>
+      <c r="E26" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="21"/>
+    </row>
+    <row r="28" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="A2:F18"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:L1"/>
+    <mergeCell ref="G2:L18"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B21:I21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
selenium added for demo
</commit_message>
<xml_diff>
--- a/src/main/resources/DemoXml/Xml File Info.xlsx
+++ b/src/main/resources/DemoXml/Xml File Info.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nabeel.Ahmed\Downloads\RAAD-Converter\src\main\resources\DemoXml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDED9166-DBED-4866-9BB3-5E7E1C12DC5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDA1084-B747-4A94-A0D8-1B7EFFFFD53B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Xml Tage With Key" sheetId="1" r:id="rId1"/>
     <sheet name="XML Schema Definition (XSD)" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -85,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="56">
   <si>
     <t>http://www.globenewswire.com/news-release/2020/02/13/1984375/0/en/Magnetic-Resonance-Imaging-MRI-Devices-and-Equipment-Industry-2015-2030-Global-Market-to-Reach-9-34B-by-2022-Rising-from-7-6B-in-2018.html</t>
   </si>
@@ -228,12 +229,78 @@
   <si>
     <t>fixed</t>
   </si>
+  <si>
+    <t>Tag Name</t>
+  </si>
+  <si>
+    <t>Parent Tag</t>
+  </si>
+  <si>
+    <t>Html Tag</t>
+  </si>
+  <si>
+    <t>itemId</t>
+  </si>
+  <si>
+    <t>Nabeel</t>
+  </si>
+  <si>
+    <t>Ahmed</t>
+  </si>
+  <si>
+    <t>Fawad</t>
+  </si>
+  <si>
+    <t>Noman</t>
+  </si>
+  <si>
+    <t>Taha</t>
+  </si>
+  <si>
+    <t>ClinicalTrial</t>
+  </si>
+  <si>
+    <t>CTRINumber</t>
+  </si>
+  <si>
+    <t>LastModifiedOn</t>
+  </si>
+  <si>
+    <t>CTRI/2019/06/019758</t>
+  </si>
+  <si>
+    <t>18/06/2019</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>PostGraduateThesis</t>
+  </si>
+  <si>
+    <t>SecondaryIDsIfAny</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>Protocol Version 7 dated 13/03/2014-Reg</t>
+  </si>
+  <si>
+    <t>SecondaryID</t>
+  </si>
+  <si>
+    <t>Identifier</t>
+  </si>
+  <si>
+    <t>Protocol Number</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,6 +378,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -454,7 +528,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -465,15 +539,25 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -507,16 +591,8 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -886,364 +962,370 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{708AC2AB-D2B5-4AF4-BD65-D93FFA26CDBB}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B21" sqref="B21:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="9" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="10" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="12"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="16"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="15"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="19"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="15"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="19"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="15"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="19"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="15"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="19"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="15"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="19"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="15"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="19"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="15"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="19"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="15"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="19"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="15"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="19"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="15"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="19"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="15"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="19"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="15"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="19"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="15"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="19"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="15"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="19"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="15"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="19"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="18"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="22"/>
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
     </row>
     <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="22"/>
-      <c r="E23" s="23" t="s">
+      <c r="C23" s="9"/>
+      <c r="E23" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="21"/>
-      <c r="E24" s="23" t="s">
+      <c r="C24" s="7"/>
+      <c r="E24" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="21"/>
-      <c r="E25" s="23" t="s">
+      <c r="C25" s="7"/>
+      <c r="E25" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="21"/>
-      <c r="E26" s="23" t="s">
+      <c r="C26" s="7"/>
+      <c r="E26" s="6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="21"/>
+      <c r="C27" s="7"/>
     </row>
     <row r="28" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="21"/>
+      <c r="C28" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="A2:F18"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:L1"/>
+    <mergeCell ref="G2:L18"/>
+    <mergeCell ref="B20:I20"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B22:I22"/>
     <mergeCell ref="B23:C23"/>
@@ -1251,15 +1333,175 @@
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B27:C27"/>
-    <mergeCell ref="A2:F18"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G1:L1"/>
-    <mergeCell ref="G2:L18"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="B21:I21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17132009-9352-453A-9F3B-B0CD5B1AB3A6}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>